<commit_message>
fix: reviewsCount 1.2k to 1200
</commit_message>
<xml_diff>
--- a/yelp.xlsx
+++ b/yelp.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,217 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>rating</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>reviewCount</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cobble Fish</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>42</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Seafood, Cocktail Bars, South Street Seaport</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sweetwater Restaurant</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>483</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>New American, Bars</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Okdongsik</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>290</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Korean, Soup, Soul Food</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fresh Salt</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>425</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bars, New American</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Debajo</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>79</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tapas Bars, Spanish, Tapas/Small Plates, Flatiron</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>nonono</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Izakaya, Cocktail Bars</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sweet Anaelle</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Peruvian, Cocktail Bars, Bushwick</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Betong - Khao Man Gai</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Thai</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>OBAO</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4200</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Vietnamese, Thai, Asian Fusion</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>R40</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>215</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Argentine, Cocktail Bars</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: code quality pep8 fine
</commit_message>
<xml_diff>
--- a/yelp.xlsx
+++ b/yelp.xlsx
@@ -458,180 +458,180 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cobble Fish</t>
+          <t>Trad Room</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.1</v>
+        <v>4.3</v>
       </c>
       <c r="C2" t="n">
-        <v>42</v>
+        <v>168</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Seafood, Cocktail Bars, South Street Seaport</t>
+          <t>Japanese,Sushi Bars,Cocktail Bars</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sweetwater Restaurant</t>
+          <t>Tradisyon</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.1</v>
+        <v>4.3</v>
       </c>
       <c r="C3" t="n">
-        <v>483</v>
+        <v>284</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>New American, Bars</t>
+          <t>Filipino</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Okdongsik</t>
+          <t>Dolly Varden</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="C4" t="n">
-        <v>290</v>
+        <v>531</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Korean, Soup, Soul Food</t>
+          <t>Cocktail Bars,New American,Breakfast &amp; Brunch</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fresh Salt</t>
+          <t>Friend Of A Farmer - Upper West Side</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="C5" t="n">
-        <v>425</v>
+        <v>35</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bars, New American</t>
+          <t>American,Comfort Food,Breakfast &amp; Brunch,Upper West Side</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Debajo</t>
+          <t>Winona’s</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>4.5</v>
       </c>
       <c r="C6" t="n">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Tapas Bars, Spanish, Tapas/Small Plates, Flatiron</t>
+          <t>American,Bedford Stuyvesant</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>nonono</t>
+          <t>Butler</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>4.2</v>
       </c>
       <c r="C7" t="n">
-        <v>1200</v>
+        <v>209</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Izakaya, Cocktail Bars</t>
+          <t>Coffee &amp; Tea,Cafes</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sweet Anaelle</t>
+          <t>Carla</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.7</v>
+        <v>4.4</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Peruvian, Cocktail Bars, Bushwick</t>
+          <t>New American,Burgers,Cocktail Bars</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Betong - Khao Man Gai</t>
+          <t>Bolivian Llama Party</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="C9" t="n">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Thai</t>
+          <t>Latin American,Sunnyside</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OBAO</t>
+          <t>5ive Spice</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>4.6</v>
       </c>
       <c r="C10" t="n">
-        <v>4200</v>
+        <v>749</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Vietnamese, Thai, Asian Fusion</t>
+          <t>Vietnamese,Tacos,Sandwiches</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>R40</t>
+          <t>Grindhaus</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="C11" t="n">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Argentine, Cocktail Bars</t>
+          <t>New American</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: excel cant insert ' char
</commit_message>
<xml_diff>
--- a/yelp.xlsx
+++ b/yelp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,183 +458,564 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Trad Room</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="C2" t="n">
-        <v>168</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Japanese,Sushi Bars,Cocktail Bars</t>
+          <t>Da Andrea - Greenwich Village</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Tradisyon</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="C3" t="n">
-        <v>284</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Filipino</t>
+          <t>Thursday Kitchen</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dolly Varden</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>531</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Cocktail Bars,New American,Breakfast &amp; Brunch</t>
+          <t>The Osprey</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Friend Of A Farmer - Upper West Side</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="C5" t="n">
-        <v>35</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>American,Comfort Food,Breakfast &amp; Brunch,Upper West Side</t>
+          <t>Antidote</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Winona’s</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C6" t="n">
-        <v>53</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>American,Bedford Stuyvesant</t>
+          <t>Ye’s Apothecary</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Butler</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>209</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Coffee &amp; Tea,Cafes</t>
+          <t>FERNS</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Carla</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C8" t="n">
-        <v>176</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>New American,Burgers,Cocktail Bars</t>
+          <t>SOBOKU</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bolivian Llama Party</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="C9" t="n">
-        <v>212</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Latin American,Sunnyside</t>
+          <t>Benemon</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5ive Spice</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>749</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Vietnamese,Tacos,Sandwiches</t>
+          <t>LoveMama</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Grindhaus</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>116</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>New American</t>
-        </is>
-      </c>
-    </row>
+          <t>Soothr</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Amélie</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Raku</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Raku</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Celestine</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Salma</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mokyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Kong Sihk Tong 港食堂</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C as in Charlie</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Lucky Rabbit Noodles</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Gair</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>The Leroy House</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Uluh</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Odd Sister</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Pomp and Circumstance</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>The Frenchman’s Dough</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>La Contenta</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Very Fresh Noodles</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Win Son</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Clover Hill</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Seamore’s Dumbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Pranakhon Thai Restaurant</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ruby’s Cafe - East Village</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Seamore’s Dumbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>The Four Horsemen</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Mikado</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>The Mayfly</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Paesano of Mulberry Street</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Theodora</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Kimura</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Thai Diner</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>The Tyger</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>The Hideaway Seaport</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Agi’s Counter</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Rosticceria Evelina</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>While We Were Young</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Wenwen</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Chama Mama - Brooklyn Heights</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Valerie</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Butler</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Ampersand</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Little Owl</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>The Little Pig</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Balthazar</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>K’Far - Brooklyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Lindens</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Al Badawi</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Torrisi</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Rule of Thirds</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>MONO+MONO</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Lillo Cucina Italiana</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Xolo</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Kanyakumari</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>David Burke TImeout Market</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>The Standard East Village</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Boutros</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Top Thai Vintage</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Sartiano’s</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Forever Thai</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Calle Dao Chelsea</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Llama Inn</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>The Standard East Village</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Boutros</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Top Thai Vintage</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Sartiano’s</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Forever Thai</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Calle Dao Chelsea</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Llama Inn</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Red Hook Tavern</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>The Consulate - Midtown</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>DOMODOMO - New York</t>
+        </is>
+      </c>
+    </row>
+    <row r="82"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>